<commit_message>
Begun work on I2C, Added VEML6070. I/O Pin Fixes.
</commit_message>
<xml_diff>
--- a/BBB IO Pins.xlsx
+++ b/BBB IO Pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\2017-18\Shared\Scarlet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\2017-18\shared\Scarlet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="60">
   <si>
     <t>Default</t>
   </si>
@@ -493,30 +493,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -618,6 +594,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,7 +1005,7 @@
   <dimension ref="B2:AB29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,32 +1024,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16"/>
-      <c r="U2" s="14" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
+      <c r="U2" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="16"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="52"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -1070,10 +1070,10 @@
       <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="54"/>
       <c r="J3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1106,10 +1106,10 @@
       <c r="W3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="X3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="13"/>
+      <c r="Y3" s="54"/>
       <c r="Z3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1121,71 +1121,73 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="10">
         <v>1</v>
       </c>
       <c r="I4" s="11">
         <v>2</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="U4" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
       <c r="X4" s="10">
         <v>1</v>
       </c>
       <c r="Y4" s="11">
         <v>2</v>
       </c>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
+      <c r="AA4" s="53"/>
+      <c r="AB4" s="53"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="8">
         <v>3</v>
       </c>
       <c r="I5" s="9">
         <v>4</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W5" s="39" t="s">
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X5" s="8">
@@ -1194,42 +1196,42 @@
       <c r="Y5" s="9">
         <v>4</v>
       </c>
-      <c r="Z5" s="53" t="s">
+      <c r="Z5" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA5" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB5" s="45"/>
+      <c r="AA5" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB5" s="37"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="8">
         <v>5</v>
       </c>
       <c r="I6" s="9">
         <v>6</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W6" s="39" t="s">
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W6" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X6" s="8">
@@ -1238,42 +1240,42 @@
       <c r="Y6" s="9">
         <v>6</v>
       </c>
-      <c r="Z6" s="53" t="s">
+      <c r="Z6" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA6" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB6" s="45"/>
+      <c r="AA6" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB6" s="37"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="8">
         <v>7</v>
       </c>
       <c r="I7" s="9">
         <v>8</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W7" s="49" t="s">
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X7" s="8">
@@ -1282,42 +1284,42 @@
       <c r="Y7" s="9">
         <v>8</v>
       </c>
-      <c r="Z7" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB7" s="45"/>
+      <c r="Z7" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="37"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="8">
         <v>9</v>
       </c>
       <c r="I8" s="9">
         <v>10</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W8" s="49" t="s">
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W8" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X8" s="8">
@@ -1326,25 +1328,25 @@
       <c r="Y8" s="9">
         <v>10</v>
       </c>
-      <c r="Z8" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB8" s="45"/>
+      <c r="Z8" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB8" s="37"/>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="31" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="33" t="s">
+      <c r="F9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="8">
@@ -1353,21 +1355,21 @@
       <c r="I9" s="9">
         <v>12</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9" s="49" t="s">
+      <c r="J9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X9" s="8">
@@ -1376,25 +1378,25 @@
       <c r="Y9" s="9">
         <v>12</v>
       </c>
-      <c r="Z9" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB9" s="45"/>
+      <c r="Z9" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB9" s="37"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="31" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="33" t="s">
+      <c r="F10" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H10" s="8">
@@ -1403,25 +1405,25 @@
       <c r="I10" s="9">
         <v>14</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="29" t="s">
+      <c r="J10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="U10" s="52" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="U10" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W10" s="49" t="s">
+      <c r="V10" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X10" s="8">
@@ -1430,23 +1432,23 @@
       <c r="Y10" s="9">
         <v>14</v>
       </c>
-      <c r="Z10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB10" s="45"/>
+      <c r="Z10" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB10" s="37"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="33" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H11" s="8">
@@ -1455,23 +1457,23 @@
       <c r="I11" s="9">
         <v>16</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="29" t="s">
+      <c r="J11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W11" s="49" t="s">
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W11" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X11" s="8">
@@ -1480,27 +1482,27 @@
       <c r="Y11" s="9">
         <v>16</v>
       </c>
-      <c r="Z11" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB11" s="45"/>
+      <c r="Z11" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB11" s="37"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="37" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H12" s="8">
@@ -1509,25 +1511,25 @@
       <c r="I12" s="9">
         <v>18</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="27" t="s">
+      <c r="J12" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W12" s="49" t="s">
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X12" s="8">
@@ -1536,27 +1538,27 @@
       <c r="Y12" s="9">
         <v>18</v>
       </c>
-      <c r="Z12" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB12" s="45"/>
+      <c r="Z12" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB12" s="37"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="37" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="33" t="s">
+      <c r="F13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="8">
@@ -1565,27 +1567,27 @@
       <c r="I13" s="9">
         <v>20</v>
       </c>
-      <c r="J13" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="27" t="s">
+      <c r="J13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="U13" s="52" t="s">
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="U13" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="V13" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W13" s="49" t="s">
+      <c r="V13" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W13" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X13" s="8">
@@ -1594,31 +1596,31 @@
       <c r="Y13" s="9">
         <v>20</v>
       </c>
-      <c r="Z13" s="53" t="s">
+      <c r="Z13" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA13" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB13" s="45"/>
+      <c r="AA13" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB13" s="37"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="33" t="s">
+      <c r="F14" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H14" s="8">
@@ -1627,29 +1629,29 @@
       <c r="I14" s="9">
         <v>22</v>
       </c>
-      <c r="J14" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="27" t="s">
+      <c r="J14" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="N14" s="42" t="s">
+      <c r="N14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="50" t="s">
+      <c r="O14" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="U14" s="51"/>
-      <c r="V14" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W14" s="39" t="s">
+      <c r="U14" s="43"/>
+      <c r="V14" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X14" s="8">
@@ -1658,23 +1660,23 @@
       <c r="Y14" s="9">
         <v>22</v>
       </c>
-      <c r="Z14" s="53" t="s">
+      <c r="Z14" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA14" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB14" s="45"/>
+      <c r="AA14" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB14" s="37"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="33" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="8">
@@ -1683,25 +1685,25 @@
       <c r="I15" s="9">
         <v>24</v>
       </c>
-      <c r="J15" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="28" t="s">
+      <c r="J15" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="42" t="s">
+      <c r="M15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="56"/>
-      <c r="O15" s="25"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W15" s="39" t="s">
+      <c r="N15" s="48"/>
+      <c r="O15" s="17"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X15" s="8">
@@ -1710,23 +1712,23 @@
       <c r="Y15" s="9">
         <v>24</v>
       </c>
-      <c r="Z15" s="53" t="s">
+      <c r="Z15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA15" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB15" s="45"/>
+      <c r="AA15" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB15" s="37"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="39" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="8">
@@ -1735,25 +1737,25 @@
       <c r="I16" s="9">
         <v>26</v>
       </c>
-      <c r="J16" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="28" t="s">
+      <c r="J16" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M16" s="42" t="s">
+      <c r="M16" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="56"/>
-      <c r="O16" s="25"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="W16" s="39" t="s">
+      <c r="N16" s="48"/>
+      <c r="O16" s="17"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W16" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X16" s="8">
@@ -1762,23 +1764,23 @@
       <c r="Y16" s="9">
         <v>26</v>
       </c>
-      <c r="Z16" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB16" s="45"/>
+      <c r="Z16" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="37"/>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="33" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H17" s="8">
@@ -1787,23 +1789,23 @@
       <c r="I17" s="9">
         <v>28</v>
       </c>
-      <c r="J17" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W17" s="39" t="s">
+      <c r="J17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W17" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X17" s="8">
@@ -1812,27 +1814,27 @@
       <c r="Y17" s="9">
         <v>28</v>
       </c>
-      <c r="Z17" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA17" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB17" s="21"/>
+      <c r="Z17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA17" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB17" s="13"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="36" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="39" t="s">
+      <c r="F18" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="8">
@@ -1841,23 +1843,23 @@
       <c r="I18" s="9">
         <v>30</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L18" s="27" t="s">
+      <c r="J18" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W18" s="39" t="s">
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W18" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X18" s="8">
@@ -1866,27 +1868,27 @@
       <c r="Y18" s="9">
         <v>30</v>
       </c>
-      <c r="Z18" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA18" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB18" s="21"/>
+      <c r="Z18" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA18" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB18" s="13"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="36" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="39" t="s">
+      <c r="F19" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H19" s="8">
@@ -1895,19 +1897,19 @@
       <c r="I19" s="9">
         <v>32</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W19" s="39" t="s">
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X19" s="8">
@@ -1916,42 +1918,42 @@
       <c r="Y19" s="9">
         <v>32</v>
       </c>
-      <c r="Z19" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA19" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB19" s="21"/>
+      <c r="Z19" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA19" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="8">
         <v>33</v>
       </c>
       <c r="I20" s="9">
         <v>34</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W20" s="39" t="s">
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W20" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X20" s="8">
@@ -1960,44 +1962,44 @@
       <c r="Y20" s="9">
         <v>34</v>
       </c>
-      <c r="Z20" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA20" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB20" s="55" t="s">
+      <c r="Z20" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA20" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB20" s="47" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
       <c r="H21" s="8">
         <v>35</v>
       </c>
       <c r="I21" s="9">
         <v>36</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W21" s="39" t="s">
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W21" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X21" s="8">
@@ -2006,44 +2008,44 @@
       <c r="Y21" s="9">
         <v>36</v>
       </c>
-      <c r="Z21" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA21" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB21" s="55" t="s">
+      <c r="Z21" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA21" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB21" s="47" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
       <c r="H22" s="8">
         <v>37</v>
       </c>
       <c r="I22" s="9">
         <v>38</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W22" s="39" t="s">
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W22" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X22" s="8">
@@ -2052,42 +2054,42 @@
       <c r="Y22" s="9">
         <v>38</v>
       </c>
-      <c r="Z22" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA22" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB22" s="21"/>
+      <c r="Z22" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
       <c r="H23" s="8">
         <v>39</v>
       </c>
       <c r="I23" s="9">
         <v>40</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W23" s="39" t="s">
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W23" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X23" s="8">
@@ -2096,23 +2098,23 @@
       <c r="Y23" s="9">
         <v>40</v>
       </c>
-      <c r="Z23" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA23" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB23" s="21"/>
+      <c r="Z23" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB23" s="13"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="33" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>0</v>
       </c>
       <c r="H24" s="8">
@@ -2121,25 +2123,25 @@
       <c r="I24" s="9">
         <v>42</v>
       </c>
-      <c r="J24" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24" s="27" t="s">
+      <c r="J24" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="42" t="s">
+      <c r="M24" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="N24" s="56"/>
-      <c r="O24" s="25"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W24" s="39" t="s">
+      <c r="N24" s="48"/>
+      <c r="O24" s="17"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X24" s="8">
@@ -2148,42 +2150,42 @@
       <c r="Y24" s="9">
         <v>42</v>
       </c>
-      <c r="Z24" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA24" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB24" s="21"/>
+      <c r="Z24" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB24" s="13"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="8">
         <v>43</v>
       </c>
       <c r="I25" s="9">
         <v>44</v>
       </c>
-      <c r="J25" s="17" t="s">
+      <c r="J25" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W25" s="39" t="s">
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X25" s="8">
@@ -2192,44 +2194,44 @@
       <c r="Y25" s="9">
         <v>44</v>
       </c>
-      <c r="Z25" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA25" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB25" s="21"/>
+      <c r="Z25" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA25" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB25" s="13"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
       <c r="H26" s="8">
         <v>45</v>
       </c>
       <c r="I26" s="9">
         <v>46</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="U26" s="40" t="s">
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="U26" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="V26" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="W26" s="39" t="s">
+      <c r="V26" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W26" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X26" s="8">
@@ -2238,13 +2240,13 @@
       <c r="Y26" s="9">
         <v>46</v>
       </c>
-      <c r="Z26" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA26" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB26" s="55" t="s">
+      <c r="Z26" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA26" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB26" s="47" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2267,23 +2269,25 @@
       <c r="T29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U29" s="20" t="s">
+      <c r="U29" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="V29" s="20"/>
+      <c r="V29" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="J21:O21"/>
-    <mergeCell ref="J22:O22"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="J19:O19"/>
@@ -2292,18 +2296,16 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="X3:Y3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Got SPI working, fixed pin chart, added raw data retrieval from sensors.
</commit_message>
<xml_diff>
--- a/BBB IO Pins.xlsx
+++ b/BBB IO Pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\2017-18\shared\Scarlet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\2017-18\Shared\Scarlet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -177,24 +177,12 @@
     <t>1_CS0</t>
   </si>
   <si>
-    <t>0_DO</t>
-  </si>
-  <si>
-    <t>0_DI</t>
-  </si>
-  <si>
     <t>0_CLK</t>
   </si>
   <si>
-    <t>1_DO</t>
-  </si>
-  <si>
     <t>1_CLK</t>
   </si>
   <si>
-    <t>1_DI</t>
-  </si>
-  <si>
     <t>1_SCL</t>
   </si>
   <si>
@@ -205,6 +193,18 @@
   </si>
   <si>
     <t>2_SDA</t>
+  </si>
+  <si>
+    <t>0_MOSI</t>
+  </si>
+  <si>
+    <t>0_MISO</t>
+  </si>
+  <si>
+    <t>1_MOSI</t>
+  </si>
+  <si>
+    <t>1_MISO</t>
   </si>
 </sst>
 </file>
@@ -595,29 +595,29 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,16 +1005,19 @@
   <dimension ref="B2:AB29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O2"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="9" width="4.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="15" width="6.42578125" customWidth="1"/>
+    <col min="2" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" customWidth="1"/>
     <col min="21" max="22" width="6.42578125" customWidth="1"/>
     <col min="23" max="23" width="7.28515625" customWidth="1"/>
@@ -1070,10 +1073,10 @@
       <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="54"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1106,10 +1109,10 @@
       <c r="W3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="54" t="s">
+      <c r="X3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="54"/>
+      <c r="Y3" s="49"/>
       <c r="Z3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1121,68 +1124,68 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="10">
         <v>1</v>
       </c>
       <c r="I4" s="11">
         <v>2</v>
       </c>
-      <c r="J4" s="56" t="s">
+      <c r="J4" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="U4" s="53" t="s">
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="U4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="53"/>
-      <c r="W4" s="53"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
       <c r="X4" s="10">
         <v>1</v>
       </c>
       <c r="Y4" s="11">
         <v>2</v>
       </c>
-      <c r="Z4" s="53" t="s">
+      <c r="Z4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="53"/>
-      <c r="AB4" s="53"/>
+      <c r="AA4" s="56"/>
+      <c r="AB4" s="56"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="8">
         <v>3</v>
       </c>
       <c r="I5" s="9">
         <v>4</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
       <c r="U5" s="43"/>
       <c r="V5" s="39" t="s">
         <v>16</v>
@@ -1205,28 +1208,28 @@
       <c r="AB5" s="37"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="8">
         <v>5</v>
       </c>
       <c r="I6" s="9">
         <v>6</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
       <c r="U6" s="43"/>
       <c r="V6" s="39" t="s">
         <v>16</v>
@@ -1249,28 +1252,28 @@
       <c r="AB6" s="37"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="8">
         <v>7</v>
       </c>
       <c r="I7" s="9">
         <v>8</v>
       </c>
-      <c r="J7" s="56" t="s">
+      <c r="J7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
       <c r="U7" s="43"/>
       <c r="V7" s="39" t="s">
         <v>16</v>
@@ -1293,28 +1296,28 @@
       <c r="AB7" s="37"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
       <c r="H8" s="8">
         <v>9</v>
       </c>
       <c r="I8" s="9">
         <v>10</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
       <c r="U8" s="43"/>
       <c r="V8" s="39" t="s">
         <v>16</v>
@@ -1494,7 +1497,7 @@
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>47</v>
@@ -1518,10 +1521,10 @@
         <v>16</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -1550,7 +1553,7 @@
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>48</v>
@@ -1577,7 +1580,7 @@
         <v>49</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -1612,10 +1615,10 @@
         <v>42</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>16</v>
@@ -1636,10 +1639,10 @@
         <v>16</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N14" s="34" t="s">
         <v>43</v>
@@ -1692,7 +1695,7 @@
         <v>16</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M15" s="34" t="s">
         <v>44</v>
@@ -1744,7 +1747,7 @@
         <v>16</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M16" s="34" t="s">
         <v>45</v>
@@ -1826,7 +1829,7 @@
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="28" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>35</v>
@@ -1850,7 +1853,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
@@ -1880,7 +1883,7 @@
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>34</v>
@@ -1897,14 +1900,14 @@
       <c r="I19" s="9">
         <v>32</v>
       </c>
-      <c r="J19" s="55" t="s">
+      <c r="J19" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
       <c r="U19" s="27"/>
       <c r="V19" s="40" t="s">
         <v>16</v>
@@ -1927,28 +1930,28 @@
       <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="8">
         <v>33</v>
       </c>
       <c r="I20" s="9">
         <v>34</v>
       </c>
-      <c r="J20" s="55" t="s">
+      <c r="J20" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
       <c r="U20" s="27"/>
       <c r="V20" s="40" t="s">
         <v>16</v>
@@ -1973,28 +1976,28 @@
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
       <c r="H21" s="8">
         <v>35</v>
       </c>
       <c r="I21" s="9">
         <v>36</v>
       </c>
-      <c r="J21" s="55" t="s">
+      <c r="J21" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
       <c r="U21" s="27"/>
       <c r="V21" s="40" t="s">
         <v>16</v>
@@ -2019,28 +2022,28 @@
       </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="8">
         <v>37</v>
       </c>
       <c r="I22" s="9">
         <v>38</v>
       </c>
-      <c r="J22" s="55" t="s">
+      <c r="J22" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
       <c r="U22" s="27"/>
       <c r="V22" s="40" t="s">
         <v>16</v>
@@ -2063,28 +2066,28 @@
       <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="8">
         <v>39</v>
       </c>
       <c r="I23" s="9">
         <v>40</v>
       </c>
-      <c r="J23" s="55" t="s">
+      <c r="J23" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
       <c r="U23" s="27"/>
       <c r="V23" s="40" t="s">
         <v>16</v>
@@ -2130,7 +2133,7 @@
         <v>16</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M24" s="34" t="s">
         <v>46</v>
@@ -2159,28 +2162,28 @@
       <c r="AB24" s="13"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
       <c r="H25" s="8">
         <v>43</v>
       </c>
       <c r="I25" s="9">
         <v>44</v>
       </c>
-      <c r="J25" s="56" t="s">
+      <c r="J25" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="53"/>
       <c r="U25" s="27"/>
       <c r="V25" s="40" t="s">
         <v>16</v>
@@ -2203,28 +2206,28 @@
       <c r="AB25" s="13"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
       <c r="H26" s="8">
         <v>45</v>
       </c>
       <c r="I26" s="9">
         <v>46</v>
       </c>
-      <c r="J26" s="56" t="s">
+      <c r="J26" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-      <c r="O26" s="56"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
       <c r="U26" s="32" t="s">
         <v>38</v>
       </c>
@@ -2269,25 +2272,18 @@
       <c r="T29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U29" s="49" t="s">
+      <c r="U29" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="V29" s="49"/>
+      <c r="V29" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="X3:Y3"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="J19:O19"/>
@@ -2301,11 +2297,18 @@
     <mergeCell ref="J23:O23"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>